<commit_message>
add file ngu phap
</commit_message>
<xml_diff>
--- a/tong hop.xlsx
+++ b/tong hop.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\support\training\Tong-hop-tieng-nhat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C952286-4B55-447E-88BF-FDF9F2E5A363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D2221B-7245-4AB2-AE50-E64AD73C18A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{89E1D6A1-2312-4BD0-BA70-A6A353BFFF01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{89E1D6A1-2312-4BD0-BA70-A6A353BFFF01}"/>
   </bookViews>
   <sheets>
     <sheet name="tong" sheetId="1" r:id="rId1"/>
     <sheet name="nghe" sheetId="2" r:id="rId2"/>
+    <sheet name="ngu phap" sheetId="3" r:id="rId3"/>
+    <sheet name="loai tu" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Các bài Minna tốt nhất cho MONDAI 1:</t>
   </si>
@@ -612,6 +614,107 @@
   </si>
   <si>
     <t>🎯 Mục tiêu: nghe hiểu tổng quát</t>
+  </si>
+  <si>
+    <t>CÁC BƯỚC LÀM BÀI DẠNG ĐIỀN TỪ TRONG ĐOẠN VĂN</t>
+  </si>
+  <si>
+    <t>BƯỚC 1: Đọc câu trước – câu sau của chỗ trống</t>
+  </si>
+  <si>
+    <t>Không cần đọc toàn bài ngay.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chỉ nhìn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1–2 câu xung quanh ô trống</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, để biết nghĩa chung.</t>
+    </r>
+  </si>
+  <si>
+    <t>BƯỚC 2: Xác định loại từ cần điền</t>
+  </si>
+  <si>
+    <t>Dựa vào:</t>
+  </si>
+  <si>
+    <t>phía trước có trợ từ gì?</t>
+  </si>
+  <si>
+    <t>phía sau là danh từ hay động từ?</t>
+  </si>
+  <si>
+    <t>có “とき”, “ので”, “から”… không?</t>
+  </si>
+  <si>
+    <t>BƯỚC 3: Loại trừ đáp án sai</t>
+  </si>
+  <si>
+    <t>BƯỚC 4: Kiểm tra nghĩa cho chắc chắn</t>
+  </si>
+  <si>
+    <t>BƯỚC 5: Đọc lại toàn đoạn để xem có bị “sai nghĩa” không</t>
+  </si>
+  <si>
+    <t>Loại từ</t>
+  </si>
+  <si>
+    <t>Dấu hiệu nhận biết</t>
+  </si>
+  <si>
+    <t>Động từ</t>
+  </si>
+  <si>
+    <t>có dạng ます, chia được thì, kết thúc bằng う/る</t>
+  </si>
+  <si>
+    <t>Danh từ</t>
+  </si>
+  <si>
+    <t>đứng trước trợ từ, sau の, không chia được</t>
+  </si>
+  <si>
+    <t>Tính từ -い</t>
+  </si>
+  <si>
+    <t>kết thúc bằng い, chia được</t>
+  </si>
+  <si>
+    <t>Tính từ -な</t>
+  </si>
+  <si>
+    <t>đứng trước N + な, không chia được</t>
+  </si>
+  <si>
+    <t>Trạng từ</t>
+  </si>
+  <si>
+    <t>kết thúc bằng に hoặc mô tả cách làm, đứng trước động từ</t>
+  </si>
+  <si>
+    <t>Dùng JLPT Sensei (đề chuẩn nhất) để kiểm tra format.</t>
+  </si>
+  <si>
+    <t>✔ Dùng Nihongo Pro để kiểm tra điểm thật của bạn.</t>
   </si>
 </sst>
 </file>
@@ -685,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -697,6 +800,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8FED63-9A69-4315-9ED6-D470C0B94771}">
   <dimension ref="A2:A70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44576681-CCF9-457E-881E-830466FC813C}">
   <dimension ref="A2:A85"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82:F83"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,4 +1577,170 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC279253-8E40-4FD9-88CE-1157B0317EA9}">
+  <dimension ref="A2:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A67E3BA-FA16-4E6F-ACA4-69D36571F656}">
+  <dimension ref="A2:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add file de 2
</commit_message>
<xml_diff>
--- a/tong hop.xlsx
+++ b/tong hop.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\support\training\Tong-hop-tieng-nhat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D2221B-7245-4AB2-AE50-E64AD73C18A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20267CD-17C1-4477-9BF3-A1E82660D442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{89E1D6A1-2312-4BD0-BA70-A6A353BFFF01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{89E1D6A1-2312-4BD0-BA70-A6A353BFFF01}"/>
   </bookViews>
   <sheets>
     <sheet name="tong" sheetId="1" r:id="rId1"/>
     <sheet name="nghe" sheetId="2" r:id="rId2"/>
     <sheet name="ngu phap" sheetId="3" r:id="rId3"/>
     <sheet name="loai tu" sheetId="4" r:id="rId4"/>
+    <sheet name="ôn" sheetId="5" r:id="rId5"/>
+    <sheet name="sap xep" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>Các bài Minna tốt nhất cho MONDAI 1:</t>
   </si>
@@ -715,13 +717,278 @@
   </si>
   <si>
     <t>✔ Dùng Nihongo Pro để kiểm tra điểm thật của bạn.</t>
+  </si>
+  <si>
+    <t>Nghe không nhìn sách (shadowing nhanh)</t>
+  </si>
+  <si>
+    <t>Bước 2 – Nghe lại + nhìn hình</t>
+  </si>
+  <si>
+    <t>Bước 3 – Nghe lần 3 + đối chiếu sách</t>
+  </si>
+  <si>
+    <t>Bước 4 – Shadowing (nhại theo)</t>
+  </si>
+  <si>
+    <t>🟦 TUẦN 1 – CỦNG CỐ NỀN + LÀM ĐỀ 1–2</t>
+  </si>
+  <si>
+    <t>Ngày 1–2: Ôn lại Minna 1–10 (từ + mẫu câu trọng tâm)</t>
+  </si>
+  <si>
+    <t>～は～です</t>
+  </si>
+  <si>
+    <t>これ／それ／あれ</t>
+  </si>
+  <si>
+    <t>この／その／あの</t>
+  </si>
+  <si>
+    <t>ここ／そこ／あそこ</t>
+  </si>
+  <si>
+    <t>～じゃありません</t>
+  </si>
+  <si>
+    <t>～ですか</t>
+  </si>
+  <si>
+    <t>なんさい／おいくつ</t>
+  </si>
+  <si>
+    <t>～の (quan hệ sở hữu)</t>
+  </si>
+  <si>
+    <t>～ます／ません／ました</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">🎧 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nghe lại bài nghe Minna bài 1–5</t>
+    </r>
+  </si>
+  <si>
+    <t>→ mục tiêu: nghe được keyword (tên, nghề, tuổi, giờ).</t>
+  </si>
+  <si>
+    <t>Ngày 3–4: Ôn lại Minna 11–17</t>
+  </si>
+  <si>
+    <t>～に / ～で</t>
+  </si>
+  <si>
+    <t>～があります／います</t>
+  </si>
+  <si>
+    <t>い形容詞／な形容詞</t>
+  </si>
+  <si>
+    <t>～てください</t>
+  </si>
+  <si>
+    <t>～てもいいです</t>
+  </si>
+  <si>
+    <t>～ています</t>
+  </si>
+  <si>
+    <t>～ましょう</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">🎧 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nghe Minna bài 6–10</t>
+    </r>
+  </si>
+  <si>
+    <t>→ bắt đầu nghe được giờ, địa điểm, chỉ đường.</t>
+  </si>
+  <si>
+    <t>Ngày 5: LÀM ĐỀ NAT-TEST SÁT THẬT – ĐỀ 1</t>
+  </si>
+  <si>
+    <t>Làm trong 50–60 phút</t>
+  </si>
+  <si>
+    <t>Sau đó tự sửa → đặc biệt là phần NGHE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nghe lại từng câu sai </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 lần</t>
+    </r>
+  </si>
+  <si>
+    <t>Ghi lại list từ chưa biết</t>
+  </si>
+  <si>
+    <t>Ngày 6–7: CHỮA ĐỀ + ÔN TIẾNG NHẬT “THỰC CHIẾN”</t>
+  </si>
+  <si>
+    <t>Ôn lại từ bị sai trong đề</t>
+  </si>
+  <si>
+    <t>Làm 1 bài nghe mini (mình có thể tạo cho bạn)</t>
+  </si>
+  <si>
+    <t>Làm 20 câu ngữ pháp trọng tâm</t>
+  </si>
+  <si>
+    <t>➡ Kết thúc tuần 1 bạn sẽ “vào guồng”, cảm giác làm đề tự tin hơn.</t>
+  </si>
+  <si>
+    <t>🟩 TUẦN 2 – TĂNG TỐC + LÀM ĐỀ</t>
+  </si>
+  <si>
+    <t>Ngày 8: Làm đề NAT-TEST số 2</t>
+  </si>
+  <si>
+    <t>→ Chấm và ghi lại lỗi.</t>
+  </si>
+  <si>
+    <t>Ngày 9–10: Luyện nghe cường độ cao</t>
+  </si>
+  <si>
+    <t>🎧 Mỗi ngày 45 phút, gồm:</t>
+  </si>
+  <si>
+    <t>1. Nghe Minna (đoạn hội thoại)</t>
+  </si>
+  <si>
+    <t>2. Nghe NAT-Test (mình có thể gửi file luyện)</t>
+  </si>
+  <si>
+    <t>3. Shadowing 10 phút</t>
+  </si>
+  <si>
+    <t>Mục tiêu tuần 2:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">➡ Nghe đúng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>60–70% câu nghe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Đủ để đậu NAT.</t>
+  </si>
+  <si>
+    <t>Ngày 11: Làm đề NAT-TEST số 3</t>
+  </si>
+  <si>
+    <t>→ Tăng tốc độ đọc hiểu + nghe.</t>
+  </si>
+  <si>
+    <t>Ngày 12–13: Làm đề NAT-TEST số 4</t>
+  </si>
+  <si>
+    <t>→ Không cần thêm đề, chỉ làm đúng 4 đề là đủ.</t>
+  </si>
+  <si>
+    <t>Ngày 14: Tổng ôn + ngủ sớm</t>
+  </si>
+  <si>
+    <t>Ôn lại từ sai</t>
+  </si>
+  <si>
+    <t>Ngữ pháp mẫu câu đơn giản</t>
+  </si>
+  <si>
+    <t>Không học cái mới</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chỉ nhìn lại </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>từ khóa nghe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (giờ, số, ngày, mua hàng, đường, người…)</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Xác định xem câu hỏi đang hỏi về cái gì (thời gian, nơi chốn, hành động,...).</t>
+  </si>
+  <si>
+    <t>2. Nhìn đáp án: loại từ nào phù hợp với cấu trúc ngữ pháp?</t>
+  </si>
+  <si>
+    <t>3. Thử lắp vào câu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,6 +1028,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -788,7 +1063,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -809,6 +1084,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1332,10 +1610,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44576681-CCF9-457E-881E-830466FC813C}">
-  <dimension ref="A2:A85"/>
+  <dimension ref="A2:A97"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,6 +1850,26 @@
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1672,7 +1970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A67E3BA-FA16-4E6F-ACA4-69D36571F656}">
   <dimension ref="A2:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1743,4 +2041,404 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A32B08-27A1-4CB0-9EDD-D3152A5833D2}">
+  <dimension ref="A3:A120"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="4"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="4"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="4"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="4"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF270EB-7C8B-4A84-ADD2-35F12BCBF346}">
+  <dimension ref="A2:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>